<commit_message>
pas-12877: small fix for nightly
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New9VIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New9VIN_CA_CHOICE.xlsx
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC1" activeCellId="1" sqref="Z1:Z1048576 AC1:AC1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>